<commit_message>
Corrected a few mistakes.
</commit_message>
<xml_diff>
--- a/Lists/Deployment Groups.xlsx
+++ b/Lists/Deployment Groups.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-Man\Documents\Brettspiele\Imperial Assault\RAIVE Reloaded\App Variant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-Man\Documents\GitHub\IA-LORAI-App\Lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6552BD7B-12D5-4082-BD6A-FBAD55E52467}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D7C8EE-2B4D-4DB1-A042-09ADFD288DDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D4A4B7AA-CD0F-479E-910F-FAFAC03BC729}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D4A4B7AA-CD0F-479E-910F-FAFAC03BC729}"/>
   </bookViews>
   <sheets>
     <sheet name="Groups" sheetId="1" r:id="rId1"/>
@@ -410,87 +410,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>#90</t>
-  </si>
-  <si>
-    <t>#91</t>
-  </si>
-  <si>
-    <t>#92</t>
-  </si>
-  <si>
-    <t>#93</t>
-  </si>
-  <si>
-    <t>#94</t>
-  </si>
-  <si>
-    <t>#95</t>
-  </si>
-  <si>
-    <t>#96</t>
-  </si>
-  <si>
-    <t>#97</t>
-  </si>
-  <si>
-    <t>#98</t>
-  </si>
-  <si>
-    <t>#99</t>
-  </si>
-  <si>
-    <t>#100</t>
-  </si>
-  <si>
-    <t>#101</t>
-  </si>
-  <si>
-    <t>#102</t>
-  </si>
-  <si>
-    <t>#103</t>
-  </si>
-  <si>
-    <t>#104</t>
-  </si>
-  <si>
-    <t>#105</t>
-  </si>
-  <si>
-    <t>#106</t>
-  </si>
-  <si>
-    <t>#107</t>
-  </si>
-  <si>
-    <t>#108</t>
-  </si>
-  <si>
-    <t>#109</t>
-  </si>
-  <si>
-    <t>#110</t>
-  </si>
-  <si>
-    <t>#111</t>
-  </si>
-  <si>
-    <t>#112</t>
-  </si>
-  <si>
-    <t>#113</t>
-  </si>
-  <si>
-    <t>#114</t>
-  </si>
-  <si>
-    <t>#115</t>
-  </si>
-  <si>
-    <t>#116</t>
-  </si>
-  <si>
     <t>DG001</t>
   </si>
   <si>
@@ -1062,6 +981,87 @@
   </si>
   <si>
     <t>Sabine Wren &amp; Zeb Orrelios</t>
+  </si>
+  <si>
+    <t>A002</t>
+  </si>
+  <si>
+    <t>A003</t>
+  </si>
+  <si>
+    <t>A004</t>
+  </si>
+  <si>
+    <t>A005</t>
+  </si>
+  <si>
+    <t>A006</t>
+  </si>
+  <si>
+    <t>A007</t>
+  </si>
+  <si>
+    <t>A008</t>
+  </si>
+  <si>
+    <t>A009</t>
+  </si>
+  <si>
+    <t>A010</t>
+  </si>
+  <si>
+    <t>A011</t>
+  </si>
+  <si>
+    <t>A012</t>
+  </si>
+  <si>
+    <t>A013</t>
+  </si>
+  <si>
+    <t>A014</t>
+  </si>
+  <si>
+    <t>A015</t>
+  </si>
+  <si>
+    <t>A016</t>
+  </si>
+  <si>
+    <t>A017</t>
+  </si>
+  <si>
+    <t>A018</t>
+  </si>
+  <si>
+    <t>A019</t>
+  </si>
+  <si>
+    <t>A020</t>
+  </si>
+  <si>
+    <t>A021</t>
+  </si>
+  <si>
+    <t>A022</t>
+  </si>
+  <si>
+    <t>A023</t>
+  </si>
+  <si>
+    <t>A024</t>
+  </si>
+  <si>
+    <t>A025</t>
+  </si>
+  <si>
+    <t>A026</t>
+  </si>
+  <si>
+    <t>A027</t>
+  </si>
+  <si>
+    <t>A028</t>
   </si>
 </sst>
 </file>
@@ -1165,29 +1165,55 @@
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="25">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1223,22 +1249,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1261,6 +1271,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1271,6 +1284,42 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1294,95 +1343,6 @@
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1397,59 +1357,59 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9EEAF312-AAD9-4FE4-8620-8FF56D0BD26B}" name="Tabelle1" displayName="Tabelle1" ref="A1:K71" totalsRowShown="0" headerRowDxfId="18" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9EEAF312-AAD9-4FE4-8620-8FF56D0BD26B}" name="Tabelle1" displayName="Tabelle1" ref="A1:K71" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A1:K71" xr:uid="{97F8D8A8-6C90-41EB-9137-DF4730CFFC1D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K71">
     <sortCondition ref="B1:B71"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{5980E0E4-305C-478B-B0E3-C5F1747CA744}" name="Group" dataCellStyle="Link"/>
-    <tableColumn id="10" xr3:uid="{3024E279-C2E6-442C-8BFC-D503A27FDC7E}" name="ID" dataDxfId="5" dataCellStyle="Link"/>
-    <tableColumn id="2" xr3:uid="{1A7BF95F-3732-45C6-8058-16AF8A18CE9D}" name="Tier" dataDxfId="6" dataCellStyle="Link"/>
-    <tableColumn id="3" xr3:uid="{7D7ED096-A47A-417F-BF55-F975A1F19927}" name="Faction" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{57CCC0FC-4D57-4B05-BBAE-AFD4FD2403CD}" name="Priority" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{B5B3371B-A99E-4108-9E21-4C10EA4B1C4D}" name="Deployment Cost" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{C7197826-16EF-486B-BE96-4AE2ABA0DD1F}" name="Reinforcement Cost" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{EEF06548-3152-4767-A7E2-63B6F6F76171}" name="Group Size" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{3024E279-C2E6-442C-8BFC-D503A27FDC7E}" name="ID" dataDxfId="22" dataCellStyle="Link"/>
+    <tableColumn id="2" xr3:uid="{1A7BF95F-3732-45C6-8058-16AF8A18CE9D}" name="Tier" dataDxfId="21" dataCellStyle="Link"/>
+    <tableColumn id="3" xr3:uid="{7D7ED096-A47A-417F-BF55-F975A1F19927}" name="Faction" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{57CCC0FC-4D57-4B05-BBAE-AFD4FD2403CD}" name="Priority" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{B5B3371B-A99E-4108-9E21-4C10EA4B1C4D}" name="Deployment Cost" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{C7197826-16EF-486B-BE96-4AE2ABA0DD1F}" name="Reinforcement Cost" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{EEF06548-3152-4767-A7E2-63B6F6F76171}" name="Group Size" dataDxfId="16"/>
     <tableColumn id="8" xr3:uid="{D165F3A5-85D0-48E8-B153-C53C3DBEC897}" name="Expansion"/>
     <tableColumn id="13" xr3:uid="{689E399B-3031-4973-91FA-A1A7BBA0B680}" name="Figure Pack"/>
-    <tableColumn id="11" xr3:uid="{95C509CB-E097-4323-803A-2FCA407D7A90}" name="Ignored Abilities" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{95C509CB-E097-4323-803A-2FCA407D7A90}" name="Ignored Abilities" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{47ACB4E3-09EF-45FD-9BA3-4D1DEE95D694}" name="Tabelle5" displayName="Tabelle5" ref="A1:J21" totalsRowShown="0" headerRowDxfId="7" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{47ACB4E3-09EF-45FD-9BA3-4D1DEE95D694}" name="Tabelle5" displayName="Tabelle5" ref="A1:J21" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:J21" xr:uid="{94A15D71-3D25-4AE9-B2F9-9E5F52428380}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J21">
     <sortCondition ref="B1:B21"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{96E730AC-E5F8-4970-8493-C67DD0043119}" name="Group" dataCellStyle="Link"/>
-    <tableColumn id="2" xr3:uid="{3CF65756-00A4-4A90-8110-8C4E89EA6B1E}" name="ID" dataDxfId="3" dataCellStyle="Link"/>
-    <tableColumn id="3" xr3:uid="{D4E0CDCF-2C66-4BEF-9D96-C940D2ACD77F}" name="Tier" dataDxfId="4" dataCellStyle="Link"/>
-    <tableColumn id="4" xr3:uid="{75ED83C7-766A-4FBD-B9AA-B68037CD1632}" name="Faction" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{BA467DF2-34A2-4E0C-B002-48E32CABD294}" name="Priority" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{4AA2CECB-2322-48B6-86CA-A7BAFE41C2B7}" name="Deployment Cost" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{C68B65A9-ED9F-47FA-B680-C550C22EF55D}" name="Group Size" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{3CF65756-00A4-4A90-8110-8C4E89EA6B1E}" name="ID" dataDxfId="12" dataCellStyle="Link"/>
+    <tableColumn id="3" xr3:uid="{D4E0CDCF-2C66-4BEF-9D96-C940D2ACD77F}" name="Tier" dataDxfId="11" dataCellStyle="Link"/>
+    <tableColumn id="4" xr3:uid="{75ED83C7-766A-4FBD-B9AA-B68037CD1632}" name="Faction" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{BA467DF2-34A2-4E0C-B002-48E32CABD294}" name="Priority" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{4AA2CECB-2322-48B6-86CA-A7BAFE41C2B7}" name="Deployment Cost" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{C68B65A9-ED9F-47FA-B680-C550C22EF55D}" name="Group Size" dataDxfId="7"/>
     <tableColumn id="8" xr3:uid="{FC8F27C0-9F32-448F-BA37-0C273BA5F4B4}" name="Expansion"/>
     <tableColumn id="11" xr3:uid="{872D22A2-EFFC-4C50-82FF-E4167504D400}" name="Figure Pack"/>
-    <tableColumn id="9" xr3:uid="{046CC7D9-B653-406D-92B3-92CD419AFD21}" name="Ignored Abilities" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{046CC7D9-B653-406D-92B3-92CD419AFD21}" name="Ignored Abilities" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8B906DE4-B26D-44C3-A765-493007D64018}" name="Tabelle4" displayName="Tabelle4" ref="A1:G29" totalsRowShown="0" headerRowDxfId="13" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8B906DE4-B26D-44C3-A765-493007D64018}" name="Tabelle4" displayName="Tabelle4" ref="A1:G29" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:G29" xr:uid="{BD257EC9-5943-4B36-B7BF-47333F7E3E48}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{9BCBEA57-9FDF-4283-B79E-525AAC4DEBDB}" name="Group" dataCellStyle="Link"/>
     <tableColumn id="2" xr3:uid="{70331FC5-CAA4-4AB3-8A81-2B124650F530}" name="ID" dataCellStyle="Link"/>
-    <tableColumn id="3" xr3:uid="{8E8E9D5D-9B04-4824-8D22-F28F754671B2}" name="Faction" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{50814B4D-B2FF-4D77-BE4D-3BC33145EDB0}" name="Threat Cost" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{A0F7755E-3A3A-4267-BB50-D3A91D5F4F12}" name="Group Size" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{8E8E9D5D-9B04-4824-8D22-F28F754671B2}" name="Faction" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{50814B4D-B2FF-4D77-BE4D-3BC33145EDB0}" name="Threat Cost" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{A0F7755E-3A3A-4267-BB50-D3A91D5F4F12}" name="Group Size" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{FFDF9332-6D50-467D-8213-39A0175F6815}" name="Expansion"/>
     <tableColumn id="7" xr3:uid="{B1BDDA16-2C83-445C-891F-DB9E54A2A93D}" name="Figure Pack" dataDxfId="0"/>
   </tableColumns>
@@ -1756,8 +1716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35153987-D984-4056-95B6-8E641839DF1E}">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1805,10 +1765,10 @@
         <v>4</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>308</v>
+        <v>281</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>247</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1816,7 +1776,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>123</v>
@@ -1840,10 +1800,10 @@
         <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>309</v>
+        <v>282</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>284</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1851,7 +1811,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>123</v>
@@ -1875,10 +1835,10 @@
         <v>33</v>
       </c>
       <c r="J3" t="s">
-        <v>309</v>
+        <v>282</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>284</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1886,7 +1846,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>123</v>
@@ -1910,10 +1870,10 @@
         <v>33</v>
       </c>
       <c r="J4" t="s">
-        <v>309</v>
+        <v>282</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>285</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1921,7 +1881,7 @@
         <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>124</v>
@@ -1936,7 +1896,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H5" s="6">
         <v>1</v>
@@ -1945,10 +1905,10 @@
         <v>33</v>
       </c>
       <c r="J5" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>292</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1956,7 +1916,7 @@
         <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>124</v>
@@ -1971,7 +1931,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H6" s="6">
         <v>1</v>
@@ -1980,10 +1940,10 @@
         <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>292</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1991,7 +1951,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>124</v>
@@ -2006,7 +1966,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H7" s="6">
         <v>1</v>
@@ -2015,10 +1975,10 @@
         <v>33</v>
       </c>
       <c r="J7" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -2026,7 +1986,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>123</v>
@@ -2041,7 +2001,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H8" s="6">
         <v>1</v>
@@ -2050,10 +2010,10 @@
         <v>33</v>
       </c>
       <c r="J8" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>262</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -2061,7 +2021,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>123</v>
@@ -2076,7 +2036,7 @@
         <v>8</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H9" s="6">
         <v>1</v>
@@ -2085,10 +2045,10 @@
         <v>33</v>
       </c>
       <c r="J9" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>262</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -2096,7 +2056,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>123</v>
@@ -2120,10 +2080,10 @@
         <v>33</v>
       </c>
       <c r="J10" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -2131,7 +2091,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>125</v>
@@ -2155,10 +2115,10 @@
         <v>33</v>
       </c>
       <c r="J11" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -2166,7 +2126,7 @@
         <v>28</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>124</v>
@@ -2181,7 +2141,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H12" s="6">
         <v>1</v>
@@ -2190,10 +2150,10 @@
         <v>33</v>
       </c>
       <c r="J12" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>293</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2201,7 +2161,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>124</v>
@@ -2216,7 +2176,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H13" s="6">
         <v>1</v>
@@ -2225,10 +2185,10 @@
         <v>33</v>
       </c>
       <c r="J13" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>293</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -2236,7 +2196,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>124</v>
@@ -2251,7 +2211,7 @@
         <v>5</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H14" s="6">
         <v>1</v>
@@ -2260,10 +2220,10 @@
         <v>33</v>
       </c>
       <c r="J14" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>294</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2271,7 +2231,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>125</v>
@@ -2286,7 +2246,7 @@
         <v>14</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H15" s="6">
         <v>1</v>
@@ -2295,10 +2255,10 @@
         <v>33</v>
       </c>
       <c r="J15" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>251</v>
+        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2306,7 +2266,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>123</v>
@@ -2330,10 +2290,10 @@
         <v>33</v>
       </c>
       <c r="J16" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -2341,7 +2301,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>191</v>
+        <v>164</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>125</v>
@@ -2365,10 +2325,10 @@
         <v>33</v>
       </c>
       <c r="J17" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -2376,7 +2336,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>192</v>
+        <v>165</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>124</v>
@@ -2391,7 +2351,7 @@
         <v>4</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H18" s="6">
         <v>1</v>
@@ -2400,10 +2360,10 @@
         <v>33</v>
       </c>
       <c r="J18" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>278</v>
+        <v>251</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -2411,7 +2371,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>123</v>
@@ -2426,7 +2386,7 @@
         <v>6</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H19" s="6">
         <v>1</v>
@@ -2435,10 +2395,10 @@
         <v>33</v>
       </c>
       <c r="J19" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>278</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -2446,7 +2406,7 @@
         <v>36</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>123</v>
@@ -2470,10 +2430,10 @@
         <v>107</v>
       </c>
       <c r="J20" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -2481,7 +2441,7 @@
         <v>37</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>123</v>
@@ -2505,10 +2465,10 @@
         <v>107</v>
       </c>
       <c r="J21" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -2516,7 +2476,7 @@
         <v>38</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>194</v>
+        <v>167</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>124</v>
@@ -2540,10 +2500,10 @@
         <v>107</v>
       </c>
       <c r="J22" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>287</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -2551,7 +2511,7 @@
         <v>39</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>123</v>
@@ -2575,10 +2535,10 @@
         <v>107</v>
       </c>
       <c r="J23" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>287</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -2586,7 +2546,7 @@
         <v>46</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>123</v>
@@ -2610,10 +2570,10 @@
         <v>108</v>
       </c>
       <c r="J24" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>283</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -2621,7 +2581,7 @@
         <v>47</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>171</v>
+        <v>144</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>125</v>
@@ -2645,10 +2605,10 @@
         <v>108</v>
       </c>
       <c r="J25" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>283</v>
+        <v>256</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -2656,7 +2616,7 @@
         <v>48</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>172</v>
+        <v>145</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>125</v>
@@ -2671,7 +2631,7 @@
         <v>10</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H26" s="6">
         <v>1</v>
@@ -2680,10 +2640,10 @@
         <v>108</v>
       </c>
       <c r="J26" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -2691,7 +2651,7 @@
         <v>49</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>123</v>
@@ -2715,10 +2675,10 @@
         <v>108</v>
       </c>
       <c r="J27" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -2726,7 +2686,7 @@
         <v>50</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>125</v>
@@ -2750,10 +2710,10 @@
         <v>108</v>
       </c>
       <c r="J28" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -2761,7 +2721,7 @@
         <v>51</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>124</v>
@@ -2776,7 +2736,7 @@
         <v>5</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H29" s="6">
         <v>1</v>
@@ -2785,10 +2745,10 @@
         <v>108</v>
       </c>
       <c r="J29" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>289</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -2796,7 +2756,7 @@
         <v>52</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>199</v>
+        <v>172</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>123</v>
@@ -2811,7 +2771,7 @@
         <v>8</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H30" s="6">
         <v>1</v>
@@ -2820,10 +2780,10 @@
         <v>108</v>
       </c>
       <c r="J30" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>289</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -2831,7 +2791,7 @@
         <v>59</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>124</v>
@@ -2846,7 +2806,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H31" s="6">
         <v>1</v>
@@ -2855,10 +2815,10 @@
         <v>109</v>
       </c>
       <c r="J31" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>295</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -2866,7 +2826,7 @@
         <v>59</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>201</v>
+        <v>174</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>124</v>
@@ -2881,7 +2841,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H32" s="6">
         <v>1</v>
@@ -2890,10 +2850,10 @@
         <v>109</v>
       </c>
       <c r="J32" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>295</v>
+        <v>268</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -2901,7 +2861,7 @@
         <v>57</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>202</v>
+        <v>175</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>124</v>
@@ -2916,7 +2876,7 @@
         <v>5</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H33" s="6">
         <v>1</v>
@@ -2925,10 +2885,10 @@
         <v>109</v>
       </c>
       <c r="J33" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>288</v>
+        <v>261</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -2936,7 +2896,7 @@
         <v>60</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>123</v>
@@ -2960,10 +2920,10 @@
         <v>109</v>
       </c>
       <c r="J34" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>296</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -2971,7 +2931,7 @@
         <v>60</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>123</v>
@@ -2995,10 +2955,10 @@
         <v>109</v>
       </c>
       <c r="J35" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>296</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -3006,7 +2966,7 @@
         <v>58</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>205</v>
+        <v>178</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>123</v>
@@ -3030,10 +2990,10 @@
         <v>109</v>
       </c>
       <c r="J36" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>291</v>
+        <v>264</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -3041,7 +3001,7 @@
         <v>69</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>124</v>
@@ -3065,10 +3025,10 @@
         <v>110</v>
       </c>
       <c r="J37" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>297</v>
+        <v>270</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -3076,7 +3036,7 @@
         <v>69</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>124</v>
@@ -3100,10 +3060,10 @@
         <v>110</v>
       </c>
       <c r="J38" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K38" s="10" t="s">
-        <v>297</v>
+        <v>270</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -3111,7 +3071,7 @@
         <v>64</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>123</v>
@@ -3135,10 +3095,10 @@
         <v>110</v>
       </c>
       <c r="J39" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -3146,7 +3106,7 @@
         <v>70</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>123</v>
@@ -3170,10 +3130,10 @@
         <v>110</v>
       </c>
       <c r="J40" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>299</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -3181,7 +3141,7 @@
         <v>70</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>123</v>
@@ -3205,10 +3165,10 @@
         <v>110</v>
       </c>
       <c r="J41" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>299</v>
+        <v>272</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -3216,7 +3176,7 @@
         <v>65</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>123</v>
@@ -3240,10 +3200,10 @@
         <v>110</v>
       </c>
       <c r="J42" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>300</v>
+        <v>273</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -3251,7 +3211,7 @@
         <v>71</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>209</v>
+        <v>182</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>124</v>
@@ -3275,10 +3235,10 @@
         <v>110</v>
       </c>
       <c r="J43" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>301</v>
+        <v>274</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
@@ -3286,7 +3246,7 @@
         <v>71</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>210</v>
+        <v>183</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>124</v>
@@ -3310,10 +3270,10 @@
         <v>110</v>
       </c>
       <c r="J44" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>301</v>
+        <v>274</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -3321,7 +3281,7 @@
         <v>66</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>211</v>
+        <v>184</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>123</v>
@@ -3345,10 +3305,10 @@
         <v>110</v>
       </c>
       <c r="J45" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>290</v>
+        <v>263</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
@@ -3356,7 +3316,7 @@
         <v>72</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>212</v>
+        <v>185</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>125</v>
@@ -3371,7 +3331,7 @@
         <v>10</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H46" s="6">
         <v>1</v>
@@ -3380,10 +3340,10 @@
         <v>110</v>
       </c>
       <c r="J46" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
@@ -3391,7 +3351,7 @@
         <v>74</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>123</v>
@@ -3406,7 +3366,7 @@
         <v>9</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H47" s="6">
         <v>1</v>
@@ -3415,10 +3375,10 @@
         <v>111</v>
       </c>
       <c r="J47" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
@@ -3426,7 +3386,7 @@
         <v>77</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>124</v>
@@ -3450,10 +3410,10 @@
         <v>111</v>
       </c>
       <c r="J48" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>302</v>
+        <v>275</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
@@ -3461,7 +3421,7 @@
         <v>77</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>124</v>
@@ -3485,10 +3445,10 @@
         <v>111</v>
       </c>
       <c r="J49" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>302</v>
+        <v>275</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
@@ -3496,7 +3456,7 @@
         <v>78</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>123</v>
@@ -3520,10 +3480,10 @@
         <v>111</v>
       </c>
       <c r="J50" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>279</v>
+        <v>252</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
@@ -3531,7 +3491,7 @@
         <v>79</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>180</v>
+        <v>153</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>123</v>
@@ -3555,10 +3515,10 @@
         <v>111</v>
       </c>
       <c r="J51" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>282</v>
+        <v>255</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
@@ -3566,7 +3526,7 @@
         <v>79</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>181</v>
+        <v>154</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>123</v>
@@ -3590,10 +3550,10 @@
         <v>111</v>
       </c>
       <c r="J52" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K52" s="10" t="s">
-        <v>282</v>
+        <v>255</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
@@ -3601,7 +3561,7 @@
         <v>76</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>125</v>
@@ -3625,10 +3585,10 @@
         <v>111</v>
       </c>
       <c r="J53" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K53" s="10" t="s">
-        <v>282</v>
+        <v>255</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
@@ -3636,7 +3596,7 @@
         <v>80</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>213</v>
+        <v>186</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>124</v>
@@ -3651,7 +3611,7 @@
         <v>4</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H54" s="6">
         <v>1</v>
@@ -3660,10 +3620,10 @@
         <v>111</v>
       </c>
       <c r="J54" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K54" s="10" t="s">
-        <v>257</v>
+        <v>230</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
@@ -3671,7 +3631,7 @@
         <v>80</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>214</v>
+        <v>187</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>124</v>
@@ -3686,7 +3646,7 @@
         <v>4</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H55" s="6">
         <v>1</v>
@@ -3695,10 +3655,10 @@
         <v>111</v>
       </c>
       <c r="J55" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K55" s="10" t="s">
-        <v>257</v>
+        <v>230</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
@@ -3706,7 +3666,7 @@
         <v>81</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>215</v>
+        <v>188</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>123</v>
@@ -3721,7 +3681,7 @@
         <v>6</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H56" s="6">
         <v>1</v>
@@ -3730,10 +3690,10 @@
         <v>111</v>
       </c>
       <c r="J56" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K56" s="10" t="s">
-        <v>257</v>
+        <v>230</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
@@ -3741,7 +3701,7 @@
         <v>88</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>124</v>
@@ -3756,7 +3716,7 @@
         <v>3</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H57" s="6">
         <v>1</v>
@@ -3765,10 +3725,10 @@
         <v>112</v>
       </c>
       <c r="J57" t="s">
+        <v>249</v>
+      </c>
+      <c r="K57" s="10" t="s">
         <v>276</v>
-      </c>
-      <c r="K57" s="10" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
@@ -3776,7 +3736,7 @@
         <v>88</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>124</v>
@@ -3791,7 +3751,7 @@
         <v>3</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H58" s="6">
         <v>1</v>
@@ -3800,10 +3760,10 @@
         <v>112</v>
       </c>
       <c r="J58" t="s">
+        <v>249</v>
+      </c>
+      <c r="K58" s="10" t="s">
         <v>276</v>
-      </c>
-      <c r="K58" s="10" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
@@ -3811,7 +3771,7 @@
         <v>87</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>124</v>
@@ -3826,7 +3786,7 @@
         <v>4</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H59" s="6">
         <v>1</v>
@@ -3835,10 +3795,10 @@
         <v>112</v>
       </c>
       <c r="J59" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K59" s="10" t="s">
-        <v>304</v>
+        <v>277</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
@@ -3846,7 +3806,7 @@
         <v>87</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>124</v>
@@ -3861,7 +3821,7 @@
         <v>4</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H60" s="6">
         <v>1</v>
@@ -3870,10 +3830,10 @@
         <v>112</v>
       </c>
       <c r="J60" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K60" s="10" t="s">
-        <v>304</v>
+        <v>277</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
@@ -3881,7 +3841,7 @@
         <v>91</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>216</v>
+        <v>189</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>124</v>
@@ -3905,10 +3865,10 @@
         <v>112</v>
       </c>
       <c r="J61" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K61" s="10" t="s">
-        <v>305</v>
+        <v>278</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
@@ -3916,7 +3876,7 @@
         <v>92</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>217</v>
+        <v>190</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>123</v>
@@ -3940,10 +3900,10 @@
         <v>112</v>
       </c>
       <c r="J62" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="K62" s="10" t="s">
-        <v>306</v>
+        <v>279</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
@@ -3951,7 +3911,7 @@
         <v>101</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>124</v>
@@ -3966,19 +3926,19 @@
         <v>5</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H63" s="6">
         <v>1</v>
       </c>
       <c r="I63" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="J63" t="s">
-        <v>310</v>
+        <v>283</v>
       </c>
       <c r="K63" s="10" t="s">
-        <v>260</v>
+        <v>233</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
@@ -3986,7 +3946,7 @@
         <v>102</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>218</v>
+        <v>191</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>124</v>
@@ -4007,13 +3967,13 @@
         <v>2</v>
       </c>
       <c r="I64" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="J64" t="s">
-        <v>311</v>
+        <v>284</v>
       </c>
       <c r="K64" s="10" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
@@ -4021,7 +3981,7 @@
         <v>103</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>219</v>
+        <v>192</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>123</v>
@@ -4042,13 +4002,13 @@
         <v>2</v>
       </c>
       <c r="I65" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="J65" t="s">
-        <v>311</v>
+        <v>284</v>
       </c>
       <c r="K65" s="10" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
@@ -4056,7 +4016,7 @@
         <v>104</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>123</v>
@@ -4071,19 +4031,19 @@
         <v>9</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H66" s="6">
         <v>1</v>
       </c>
       <c r="I66" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="J66" t="s">
-        <v>312</v>
+        <v>285</v>
       </c>
       <c r="K66" s="10" t="s">
-        <v>252</v>
+        <v>225</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
@@ -4091,7 +4051,7 @@
         <v>105</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>124</v>
@@ -4106,19 +4066,19 @@
         <v>2</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H67" s="6">
         <v>1</v>
       </c>
       <c r="I67" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="J67" t="s">
-        <v>313</v>
+        <v>286</v>
       </c>
       <c r="K67" s="10" t="s">
-        <v>307</v>
+        <v>280</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
@@ -4126,7 +4086,7 @@
         <v>106</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>124</v>
@@ -4141,19 +4101,19 @@
         <v>3</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="H68" s="6">
         <v>1</v>
       </c>
       <c r="I68" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="J68" t="s">
-        <v>313</v>
+        <v>286</v>
       </c>
       <c r="K68" s="10" t="s">
-        <v>274</v>
+        <v>247</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
@@ -4161,7 +4121,7 @@
         <v>113</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>124</v>
@@ -4182,13 +4142,13 @@
         <v>2</v>
       </c>
       <c r="I69" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="J69" t="s">
-        <v>314</v>
+        <v>287</v>
       </c>
       <c r="K69" s="10" t="s">
-        <v>272</v>
+        <v>245</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
@@ -4196,7 +4156,7 @@
         <v>114</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>123</v>
@@ -4217,48 +4177,48 @@
         <v>2</v>
       </c>
       <c r="I70" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="J70" t="s">
-        <v>314</v>
+        <v>287</v>
       </c>
       <c r="K70" s="10" t="s">
-        <v>272</v>
+        <v>245</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>223</v>
+        <v>196</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="E71" s="6">
         <v>2</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="H71" s="6">
         <v>1</v>
       </c>
       <c r="I71" t="s">
-        <v>246</v>
+        <v>219</v>
       </c>
       <c r="J71" t="s">
-        <v>246</v>
+        <v>219</v>
       </c>
       <c r="K71" s="10" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -4346,8 +4306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA4D9C37-CF56-4979-8AC6-3AEEFE784A44}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4389,10 +4349,10 @@
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>308</v>
+        <v>281</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>247</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -4400,7 +4360,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>125</v>
@@ -4421,10 +4381,10 @@
         <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>325</v>
+        <v>298</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -4432,7 +4392,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>125</v>
@@ -4453,10 +4413,10 @@
         <v>33</v>
       </c>
       <c r="I3" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>258</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -4464,7 +4424,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>226</v>
+        <v>199</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>125</v>
@@ -4485,10 +4445,10 @@
         <v>33</v>
       </c>
       <c r="I4" t="s">
-        <v>322</v>
+        <v>295</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -4496,7 +4456,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>227</v>
+        <v>200</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>125</v>
@@ -4517,10 +4477,10 @@
         <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>329</v>
+        <v>302</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>280</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -4528,7 +4488,7 @@
         <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>228</v>
+        <v>201</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>125</v>
@@ -4549,10 +4509,10 @@
         <v>107</v>
       </c>
       <c r="I6" t="s">
-        <v>327</v>
+        <v>300</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>275</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -4560,7 +4520,7 @@
         <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>229</v>
+        <v>202</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>125</v>
@@ -4581,10 +4541,10 @@
         <v>107</v>
       </c>
       <c r="I7" t="s">
-        <v>317</v>
+        <v>290</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>253</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -4592,7 +4552,7 @@
         <v>53</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>230</v>
+        <v>203</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>123</v>
@@ -4613,10 +4573,10 @@
         <v>108</v>
       </c>
       <c r="I8" t="s">
-        <v>319</v>
+        <v>292</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>259</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -4624,7 +4584,7 @@
         <v>54</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>231</v>
+        <v>204</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>123</v>
@@ -4645,10 +4605,10 @@
         <v>108</v>
       </c>
       <c r="I9" t="s">
-        <v>321</v>
+        <v>294</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>263</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -4656,7 +4616,7 @@
         <v>55</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>232</v>
+        <v>205</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>123</v>
@@ -4677,10 +4637,10 @@
         <v>109</v>
       </c>
       <c r="I10" t="s">
-        <v>316</v>
+        <v>289</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -4688,7 +4648,7 @@
         <v>56</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>233</v>
+        <v>206</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>123</v>
@@ -4709,10 +4669,10 @@
         <v>109</v>
       </c>
       <c r="I11" t="s">
-        <v>318</v>
+        <v>291</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>254</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -4720,7 +4680,7 @@
         <v>67</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>234</v>
+        <v>207</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>123</v>
@@ -4741,10 +4701,10 @@
         <v>110</v>
       </c>
       <c r="I12" t="s">
-        <v>326</v>
+        <v>299</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>273</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -4752,7 +4712,7 @@
         <v>68</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>235</v>
+        <v>208</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>123</v>
@@ -4773,10 +4733,10 @@
         <v>110</v>
       </c>
       <c r="I13" t="s">
-        <v>310</v>
+        <v>283</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>256</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -4784,7 +4744,7 @@
         <v>75</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>236</v>
+        <v>209</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>123</v>
@@ -4805,10 +4765,10 @@
         <v>111</v>
       </c>
       <c r="I14" t="s">
-        <v>320</v>
+        <v>293</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>261</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -4816,7 +4776,7 @@
         <v>82</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>237</v>
+        <v>210</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>123</v>
@@ -4837,10 +4797,10 @@
         <v>111</v>
       </c>
       <c r="I15" t="s">
-        <v>328</v>
+        <v>301</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>277</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -4848,7 +4808,7 @@
         <v>89</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>238</v>
+        <v>211</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>123</v>
@@ -4869,10 +4829,10 @@
         <v>112</v>
       </c>
       <c r="I16" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>286</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -4880,7 +4840,7 @@
         <v>90</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>239</v>
+        <v>212</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>123</v>
@@ -4901,10 +4861,10 @@
         <v>112</v>
       </c>
       <c r="I17" t="s">
-        <v>324</v>
+        <v>297</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>270</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -4912,7 +4872,7 @@
         <v>98</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>240</v>
+        <v>213</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>123</v>
@@ -4930,13 +4890,13 @@
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="I18" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>265</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -4944,7 +4904,7 @@
         <v>99</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>241</v>
+        <v>214</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>124</v>
@@ -4962,13 +4922,13 @@
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="I19" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>248</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -4976,7 +4936,7 @@
         <v>100</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>244</v>
+        <v>217</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>123</v>
@@ -4994,21 +4954,21 @@
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="I20" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>255</v>
+        <v>228</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>267</v>
+        <v>240</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>123</v>
@@ -5026,13 +4986,13 @@
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="I21" t="s">
-        <v>323</v>
+        <v>296</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -5071,13 +5031,13 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" style="6"/>
     <col min="4" max="4" width="12.44140625" style="6" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" style="6" customWidth="1"/>
@@ -5105,7 +5065,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>308</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -5113,7 +5073,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>242</v>
+        <v>215</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>32</v>
@@ -5128,7 +5088,7 @@
         <v>33</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -5136,7 +5096,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>127</v>
+        <v>318</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>32</v>
@@ -5151,7 +5111,7 @@
         <v>33</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>339</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -5159,7 +5119,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>128</v>
+        <v>319</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>32</v>
@@ -5174,7 +5134,7 @@
         <v>33</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>338</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -5182,7 +5142,7 @@
         <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>129</v>
+        <v>320</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>32</v>
@@ -5205,7 +5165,7 @@
         <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>130</v>
+        <v>321</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>32</v>
@@ -5220,7 +5180,7 @@
         <v>33</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>340</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -5228,7 +5188,7 @@
         <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>131</v>
+        <v>322</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>32</v>
@@ -5243,7 +5203,7 @@
         <v>107</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -5251,7 +5211,7 @@
         <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>132</v>
+        <v>323</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>32</v>
@@ -5266,7 +5226,7 @@
         <v>107</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -5274,7 +5234,7 @@
         <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>133</v>
+        <v>324</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>32</v>
@@ -5289,7 +5249,7 @@
         <v>108</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>342</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -5297,7 +5257,7 @@
         <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>134</v>
+        <v>325</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>32</v>
@@ -5312,7 +5272,7 @@
         <v>108</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>337</v>
+        <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -5320,7 +5280,7 @@
         <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>135</v>
+        <v>326</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>32</v>
@@ -5343,7 +5303,7 @@
         <v>62</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>136</v>
+        <v>327</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>32</v>
@@ -5366,7 +5326,7 @@
         <v>63</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>137</v>
+        <v>328</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>32</v>
@@ -5389,7 +5349,7 @@
         <v>73</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>138</v>
+        <v>329</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>32</v>
@@ -5412,7 +5372,7 @@
         <v>84</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>139</v>
+        <v>330</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>32</v>
@@ -5427,7 +5387,7 @@
         <v>112</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>343</v>
+        <v>316</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -5435,7 +5395,7 @@
         <v>85</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>140</v>
+        <v>331</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>32</v>
@@ -5450,7 +5410,7 @@
         <v>112</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>343</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -5458,7 +5418,7 @@
         <v>86</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>141</v>
+        <v>332</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>32</v>
@@ -5473,7 +5433,7 @@
         <v>112</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -5481,7 +5441,7 @@
         <v>83</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>142</v>
+        <v>333</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>32</v>
@@ -5496,7 +5456,7 @@
         <v>112</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -5504,7 +5464,7 @@
         <v>94</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>143</v>
+        <v>334</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>32</v>
@@ -5516,10 +5476,10 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>332</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -5527,7 +5487,7 @@
         <v>96</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>144</v>
+        <v>335</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>32</v>
@@ -5539,10 +5499,10 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>333</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -5550,7 +5510,7 @@
         <v>97</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>145</v>
+        <v>336</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>32</v>
@@ -5562,10 +5522,10 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>333</v>
+        <v>306</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -5573,7 +5533,7 @@
         <v>93</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>146</v>
+        <v>337</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>32</v>
@@ -5585,10 +5545,10 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>334</v>
+        <v>307</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -5596,7 +5556,7 @@
         <v>115</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>147</v>
+        <v>338</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>32</v>
@@ -5608,10 +5568,10 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>334</v>
+        <v>307</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -5619,7 +5579,7 @@
         <v>116</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>148</v>
+        <v>339</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>32</v>
@@ -5631,10 +5591,10 @@
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>335</v>
+        <v>308</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -5642,7 +5602,7 @@
         <v>117</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>149</v>
+        <v>340</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>32</v>
@@ -5654,10 +5614,10 @@
         <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>335</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -5665,7 +5625,7 @@
         <v>118</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>150</v>
+        <v>341</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>32</v>
@@ -5677,10 +5637,10 @@
         <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>336</v>
+        <v>309</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -5688,7 +5648,7 @@
         <v>119</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>151</v>
+        <v>342</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>32</v>
@@ -5700,10 +5660,10 @@
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>337</v>
+        <v>310</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -5711,7 +5671,7 @@
         <v>120</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>152</v>
+        <v>343</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>32</v>
@@ -5723,10 +5683,10 @@
         <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>338</v>
+        <v>311</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -5734,7 +5694,7 @@
         <v>122</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>153</v>
+        <v>344</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>32</v>
@@ -5746,10 +5706,10 @@
         <v>3</v>
       </c>
       <c r="F29" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>339</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>